<commit_message>
fixed grade for styling
</commit_message>
<xml_diff>
--- a/Doc/SRS/SRS Grade Rubric.xlsx
+++ b/Doc/SRS/SRS Grade Rubric.xlsx
@@ -670,8 +670,8 @@
   </sheetPr>
   <dimension ref="A1:C82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -806,19 +806,15 @@
       <c r="A14" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B14" s="6">
-        <v>0</v>
-      </c>
-      <c r="C14" s="6">
-        <v>0</v>
-      </c>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
     </row>
     <row r="15" spans="1:3" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>6</v>
       </c>
       <c r="B15" s="10">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C15" s="11">
         <v>8</v>
@@ -1348,7 +1344,7 @@
         <v>45</v>
       </c>
       <c r="B71" s="16">
-        <v>97.5</v>
+        <v>98.5</v>
       </c>
       <c r="C71" s="17">
         <v>100</v>

</xml_diff>